<commit_message>
added some things in mis measurements and changed dates of diameter measurements
</commit_message>
<xml_diff>
--- a/data/miscellaneousMonitoring/2024MiscellaneousMonitoring.xlsx
+++ b/data/miscellaneousMonitoring/2024MiscellaneousMonitoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/miscellaneousMonitoring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4044D2C7-21DC-3B44-8149-E25374E2297A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325596F1-4621-AD45-856A-90F7B4057B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31420" yWindow="-1380" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phenological_monitoring" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2535" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2536" uniqueCount="666">
   <si>
     <t>tree_ID</t>
   </si>
@@ -2030,7 +2030,10 @@
     <t>178_light_stress</t>
   </si>
   <si>
-    <t>177_mildew</t>
+    <t>2024_177_mildew</t>
+  </si>
+  <si>
+    <t>2025_121_mildew</t>
   </si>
 </sst>
 </file>
@@ -2521,10 +2524,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -2900,24 +2902,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J631"/>
+  <dimension ref="A1:K631"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D17" sqref="D17"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="10.83203125" style="2"/>
-    <col min="7" max="7" width="16.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2945,8 +2945,11 @@
       <c r="J1" s="1" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K1" s="1" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2966,7 +2969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2986,7 +2989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -3006,7 +3009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -3026,7 +3029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -3046,7 +3049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3066,7 +3069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -3086,7 +3089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -3106,7 +3109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -3126,7 +3129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -3146,7 +3149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -3166,7 +3169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -3186,7 +3189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -3206,7 +3209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -3226,7 +3229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -3246,7 +3249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -3286,7 +3289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -3326,7 +3329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -3366,7 +3369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -3406,7 +3409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -3446,7 +3449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -3486,7 +3489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -3526,7 +3529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -3566,7 +3569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -3606,7 +3609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -3646,7 +3649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -3686,7 +3689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -3726,7 +3729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -3766,7 +3769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -3806,7 +3809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -3846,7 +3849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -3866,7 +3869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>57</v>
       </c>
@@ -3886,7 +3889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>58</v>
       </c>
@@ -3906,7 +3909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -3926,7 +3929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>60</v>
       </c>
@@ -3946,7 +3949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>61</v>
       </c>
@@ -3966,7 +3969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>62</v>
       </c>
@@ -3986,7 +3989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>63</v>
       </c>
@@ -4006,7 +4009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>64</v>
       </c>
@@ -4026,7 +4029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>65</v>
       </c>
@@ -4046,7 +4049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>66</v>
       </c>
@@ -4066,7 +4069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>67</v>
       </c>
@@ -4086,7 +4089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>68</v>
       </c>
@@ -4106,7 +4109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>69</v>
       </c>
@@ -4126,7 +4129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>70</v>
       </c>
@@ -4145,8 +4148,11 @@
       <c r="J61" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>71</v>
       </c>
@@ -4166,7 +4172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>73</v>
       </c>
@@ -4186,7 +4192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>74</v>
       </c>
@@ -4226,7 +4232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>76</v>
       </c>
@@ -4266,7 +4272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>78</v>
       </c>
@@ -4306,7 +4312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>80</v>
       </c>
@@ -4326,7 +4332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>81</v>
       </c>
@@ -4366,7 +4372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>83</v>
       </c>
@@ -4406,7 +4412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>85</v>
       </c>
@@ -4446,7 +4452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>87</v>
       </c>
@@ -4486,7 +4492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>90</v>
       </c>
@@ -4526,7 +4532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>92</v>
       </c>
@@ -4546,7 +4552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>93</v>
       </c>
@@ -4566,7 +4572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>94</v>
       </c>
@@ -4586,7 +4592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>95</v>
       </c>
@@ -4606,7 +4612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>96</v>
       </c>
@@ -4626,7 +4632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>97</v>
       </c>
@@ -4646,7 +4652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>98</v>
       </c>
@@ -4665,8 +4671,11 @@
       <c r="J87">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>99</v>
       </c>
@@ -4685,8 +4694,11 @@
       <c r="J88" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K88" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>100</v>
       </c>
@@ -4706,7 +4718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>101</v>
       </c>
@@ -4726,7 +4738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>102</v>
       </c>
@@ -4746,7 +4758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>103</v>
       </c>
@@ -4763,7 +4775,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="93" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>106</v>
       </c>
@@ -4780,7 +4792,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="94" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>107</v>
       </c>
@@ -4797,7 +4809,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="95" spans="1:10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>108</v>
       </c>
@@ -4814,7 +4826,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="96" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>109</v>
       </c>
@@ -4831,7 +4843,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="97" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>110</v>
       </c>
@@ -4865,7 +4877,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="99" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>112</v>
       </c>
@@ -4899,7 +4911,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="101" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>114</v>
       </c>
@@ -4933,7 +4945,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="103" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>116</v>
       </c>
@@ -4967,7 +4979,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="105" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>118</v>
       </c>
@@ -5001,7 +5013,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>120</v>
       </c>
@@ -5035,7 +5047,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="109" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>122</v>
       </c>
@@ -5069,7 +5081,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="111" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>124</v>
       </c>
@@ -5103,7 +5115,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="113" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>126</v>
       </c>
@@ -5143,7 +5155,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="115" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>128</v>
       </c>
@@ -5177,7 +5189,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="117" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>130</v>
       </c>
@@ -5194,7 +5206,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="118" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>131</v>
       </c>
@@ -5228,7 +5240,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="120" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>133</v>
       </c>
@@ -5262,7 +5274,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="122" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>135</v>
       </c>
@@ -5296,7 +5308,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="124" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>137</v>
       </c>
@@ -5330,7 +5342,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="126" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>139</v>
       </c>
@@ -5364,7 +5376,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="128" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>141</v>
       </c>
@@ -5398,7 +5410,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="130" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>143</v>
       </c>
@@ -5432,7 +5444,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="132" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>145</v>
       </c>
@@ -5466,7 +5478,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="134" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>147</v>
       </c>
@@ -5500,7 +5512,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="136" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>149</v>
       </c>
@@ -5534,7 +5546,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="138" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>151</v>
       </c>
@@ -5568,7 +5580,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="140" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>153</v>
       </c>
@@ -5585,7 +5597,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="141" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>154</v>
       </c>
@@ -5619,7 +5631,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="143" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>156</v>
       </c>
@@ -5653,7 +5665,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="145" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>158</v>
       </c>
@@ -5687,7 +5699,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="147" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>160</v>
       </c>
@@ -5721,7 +5733,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="149" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>162</v>
       </c>
@@ -5755,7 +5767,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="151" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>164</v>
       </c>
@@ -5789,7 +5801,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="153" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>166</v>
       </c>
@@ -5823,7 +5835,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="155" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>168</v>
       </c>
@@ -5857,7 +5869,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="157" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>170</v>
       </c>
@@ -5891,7 +5903,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="159" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>172</v>
       </c>
@@ -5925,7 +5937,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="161" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>174</v>
       </c>
@@ -5959,7 +5971,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="163" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>176</v>
       </c>
@@ -5993,7 +6005,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="165" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>178</v>
       </c>
@@ -6027,7 +6039,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="167" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>180</v>
       </c>
@@ -6061,7 +6073,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="169" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>182</v>
       </c>
@@ -6095,7 +6107,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="171" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>184</v>
       </c>
@@ -6129,7 +6141,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="173" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>186</v>
       </c>
@@ -6163,7 +6175,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="175" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>188</v>
       </c>
@@ -6197,7 +6209,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="177" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>190</v>
       </c>
@@ -6231,7 +6243,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="179" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>192</v>
       </c>
@@ -6265,7 +6277,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="181" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>194</v>
       </c>
@@ -6299,7 +6311,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="183" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>198</v>
       </c>
@@ -6333,7 +6345,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="185" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>200</v>
       </c>
@@ -6367,7 +6379,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="187" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>202</v>
       </c>
@@ -6384,7 +6396,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="188" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>203</v>
       </c>
@@ -6418,7 +6430,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="190" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>205</v>
       </c>
@@ -6452,7 +6464,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="192" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>207</v>
       </c>
@@ -6486,7 +6498,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="194" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>209</v>
       </c>
@@ -6520,7 +6532,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="196" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>211</v>
       </c>
@@ -6554,7 +6566,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="198" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>213</v>
       </c>
@@ -6588,7 +6600,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="200" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>215</v>
       </c>
@@ -6622,7 +6634,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="202" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>217</v>
       </c>
@@ -6656,7 +6668,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="204" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>219</v>
       </c>
@@ -6690,7 +6702,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="206" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>221</v>
       </c>
@@ -6724,7 +6736,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="208" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>223</v>
       </c>
@@ -6758,7 +6770,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="210" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>225</v>
       </c>
@@ -6775,7 +6787,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="211" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>226</v>
       </c>
@@ -6809,7 +6821,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="213" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>228</v>
       </c>
@@ -6843,7 +6855,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="215" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>230</v>
       </c>
@@ -6877,7 +6889,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="217" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>232</v>
       </c>
@@ -6911,7 +6923,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="219" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>234</v>
       </c>
@@ -6945,7 +6957,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="221" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>236</v>
       </c>
@@ -6979,7 +6991,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="223" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>238</v>
       </c>
@@ -7013,7 +7025,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="225" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>240</v>
       </c>
@@ -7047,7 +7059,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="227" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>242</v>
       </c>
@@ -7081,7 +7093,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="229" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>244</v>
       </c>
@@ -7115,7 +7127,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="231" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>246</v>
       </c>
@@ -7149,7 +7161,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="233" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>248</v>
       </c>
@@ -7183,7 +7195,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="235" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>250</v>
       </c>
@@ -7217,7 +7229,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="237" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>252</v>
       </c>
@@ -7251,7 +7263,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="239" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>254</v>
       </c>
@@ -7285,7 +7297,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="241" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>256</v>
       </c>
@@ -7319,7 +7331,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="243" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>258</v>
       </c>
@@ -7353,7 +7365,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="245" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>260</v>
       </c>
@@ -7387,7 +7399,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="247" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>262</v>
       </c>
@@ -7421,7 +7433,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="249" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>264</v>
       </c>
@@ -7455,7 +7467,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="251" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>266</v>
       </c>
@@ -7489,7 +7501,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="253" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>268</v>
       </c>
@@ -7523,7 +7535,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="255" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>270</v>
       </c>
@@ -7557,7 +7569,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="257" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>272</v>
       </c>
@@ -7574,7 +7586,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="258" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>273</v>
       </c>
@@ -7608,7 +7620,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="260" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>275</v>
       </c>
@@ -7642,7 +7654,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="262" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>277</v>
       </c>
@@ -7676,7 +7688,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="264" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>279</v>
       </c>
@@ -7710,7 +7722,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="266" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>281</v>
       </c>
@@ -7744,7 +7756,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="268" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>283</v>
       </c>
@@ -7778,7 +7790,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="270" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>285</v>
       </c>
@@ -7812,7 +7824,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="272" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>287</v>
       </c>
@@ -7846,7 +7858,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="274" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>291</v>
       </c>
@@ -7880,7 +7892,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="276" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>293</v>
       </c>
@@ -7914,7 +7926,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="278" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>295</v>
       </c>
@@ -7954,7 +7966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>297</v>
       </c>
@@ -7971,7 +7983,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="281" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>298</v>
       </c>
@@ -8005,7 +8017,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="283" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>300</v>
       </c>
@@ -8039,7 +8051,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="285" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>302</v>
       </c>
@@ -8073,7 +8085,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="287" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>304</v>
       </c>
@@ -8107,7 +8119,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="289" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>306</v>
       </c>
@@ -8141,7 +8153,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="291" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>308</v>
       </c>
@@ -8175,7 +8187,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="293" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>310</v>
       </c>
@@ -8215,7 +8227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>312</v>
       </c>
@@ -8249,7 +8261,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="297" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>314</v>
       </c>
@@ -8283,7 +8295,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="299" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>316</v>
       </c>
@@ -8317,7 +8329,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="301" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>318</v>
       </c>
@@ -8351,7 +8363,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="303" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>320</v>
       </c>
@@ -8385,7 +8397,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="305" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>322</v>
       </c>
@@ -8419,7 +8431,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="307" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>324</v>
       </c>
@@ -8453,7 +8465,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="309" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>326</v>
       </c>
@@ -8487,7 +8499,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="311" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>328</v>
       </c>
@@ -8521,7 +8533,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="313" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>330</v>
       </c>
@@ -8555,7 +8567,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="315" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>332</v>
       </c>
@@ -8589,7 +8601,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="317" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>334</v>
       </c>
@@ -8623,7 +8635,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="319" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>336</v>
       </c>
@@ -8657,7 +8669,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="321" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>338</v>
       </c>
@@ -8691,7 +8703,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="323" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>340</v>
       </c>
@@ -8725,7 +8737,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="325" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>342</v>
       </c>
@@ -8759,7 +8771,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="327" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>344</v>
       </c>
@@ -8776,7 +8788,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="328" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>345</v>
       </c>
@@ -8810,7 +8822,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="330" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>347</v>
       </c>
@@ -8844,7 +8856,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="332" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>349</v>
       </c>
@@ -8878,7 +8890,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="334" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>351</v>
       </c>
@@ -8912,7 +8924,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="336" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>353</v>
       </c>
@@ -8946,7 +8958,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="338" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>355</v>
       </c>
@@ -8980,7 +8992,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="340" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>357</v>
       </c>
@@ -9014,7 +9026,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="342" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>359</v>
       </c>
@@ -9048,7 +9060,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="344" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>361</v>
       </c>
@@ -9082,7 +9094,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="346" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>363</v>
       </c>
@@ -9116,7 +9128,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="348" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>365</v>
       </c>
@@ -9150,7 +9162,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="350" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>367</v>
       </c>
@@ -9167,7 +9179,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="351" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>368</v>
       </c>
@@ -9201,7 +9213,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="353" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>370</v>
       </c>
@@ -9235,7 +9247,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="355" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>372</v>
       </c>
@@ -9269,7 +9281,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="357" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>374</v>
       </c>
@@ -9303,7 +9315,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="359" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>376</v>
       </c>
@@ -9337,7 +9349,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="361" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>378</v>
       </c>
@@ -9371,7 +9383,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="363" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>382</v>
       </c>
@@ -9405,7 +9417,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="365" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>384</v>
       </c>
@@ -9439,7 +9451,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="367" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>386</v>
       </c>
@@ -9473,7 +9485,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="369" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>388</v>
       </c>
@@ -9513,7 +9525,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="371" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>390</v>
       </c>
@@ -9547,7 +9559,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="373" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>392</v>
       </c>
@@ -9581,7 +9593,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="375" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>394</v>
       </c>
@@ -9615,7 +9627,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="377" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>396</v>
       </c>
@@ -9649,7 +9661,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="379" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>398</v>
       </c>
@@ -9689,7 +9701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="381" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>400</v>
       </c>
@@ -9723,7 +9735,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="383" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>402</v>
       </c>
@@ -9757,7 +9769,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="385" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>404</v>
       </c>
@@ -9791,7 +9803,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="387" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>406</v>
       </c>
@@ -9828,7 +9840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="389" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>408</v>
       </c>
@@ -9862,7 +9874,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="391" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>410</v>
       </c>
@@ -9902,7 +9914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="393" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>412</v>
       </c>
@@ -9939,7 +9951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="395" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
         <v>414</v>
       </c>
@@ -9973,7 +9985,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="397" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>416</v>
       </c>
@@ -9990,7 +10002,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="398" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>417</v>
       </c>
@@ -10024,7 +10036,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="400" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>419</v>
       </c>
@@ -10058,7 +10070,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="402" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>421</v>
       </c>
@@ -10095,7 +10107,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="404" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>423</v>
       </c>
@@ -10129,7 +10141,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="406" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>425</v>
       </c>
@@ -10163,7 +10175,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="408" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>427</v>
       </c>
@@ -10197,7 +10209,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="410" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>429</v>
       </c>
@@ -10231,7 +10243,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="412" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>431</v>
       </c>
@@ -10265,7 +10277,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="414" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>433</v>
       </c>
@@ -10299,7 +10311,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="416" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>435</v>
       </c>
@@ -10333,7 +10345,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="418" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>437</v>
       </c>
@@ -10367,7 +10379,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="420" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>439</v>
       </c>
@@ -10384,7 +10396,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="421" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
         <v>440</v>
       </c>
@@ -10418,7 +10430,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="423" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
         <v>442</v>
       </c>
@@ -10452,7 +10464,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="425" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
         <v>444</v>
       </c>
@@ -10489,7 +10501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="427" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
         <v>446</v>
       </c>
@@ -10523,7 +10535,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="429" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
         <v>448</v>
       </c>
@@ -10560,7 +10572,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="431" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
         <v>450</v>
       </c>
@@ -10594,7 +10606,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="433" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
         <v>452</v>
       </c>
@@ -10628,7 +10640,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="435" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
         <v>454</v>
       </c>
@@ -10662,7 +10674,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="437" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
         <v>456</v>
       </c>
@@ -10696,7 +10708,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="439" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
         <v>458</v>
       </c>
@@ -10730,7 +10742,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="441" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
         <v>460</v>
       </c>
@@ -10767,7 +10779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="443" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
         <v>462</v>
       </c>
@@ -10801,7 +10813,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="445" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
         <v>464</v>
       </c>
@@ -10835,7 +10847,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="447" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
         <v>466</v>
       </c>
@@ -10869,7 +10881,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="449" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
         <v>468</v>
       </c>
@@ -10903,7 +10915,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="451" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
         <v>470</v>
       </c>
@@ -10940,7 +10952,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="453" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
         <v>474</v>
       </c>
@@ -10974,7 +10986,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="455" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
         <v>476</v>
       </c>
@@ -11008,7 +11020,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="457" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
         <v>478</v>
       </c>
@@ -11042,7 +11054,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="459" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A459" t="s">
         <v>480</v>
       </c>
@@ -11076,7 +11088,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="461" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A461" t="s">
         <v>482</v>
       </c>
@@ -11110,7 +11122,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="463" spans="1:7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A463" t="s">
         <v>484</v>
       </c>
@@ -11144,7 +11156,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="465" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
         <v>486</v>
       </c>
@@ -11161,7 +11173,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="466" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
         <v>487</v>
       </c>
@@ -11195,7 +11207,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="468" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
         <v>489</v>
       </c>
@@ -11229,7 +11241,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="470" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
         <v>491</v>
       </c>
@@ -11263,7 +11275,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="472" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
         <v>493</v>
       </c>
@@ -11297,7 +11309,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="474" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A474" t="s">
         <v>495</v>
       </c>
@@ -11331,7 +11343,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="476" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A476" t="s">
         <v>497</v>
       </c>
@@ -11365,7 +11377,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="478" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A478" t="s">
         <v>499</v>
       </c>
@@ -11399,7 +11411,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="480" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A480" t="s">
         <v>501</v>
       </c>
@@ -11433,7 +11445,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="482" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A482" t="s">
         <v>503</v>
       </c>
@@ -11467,7 +11479,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="484" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A484" t="s">
         <v>505</v>
       </c>
@@ -11501,7 +11513,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="486" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A486" t="s">
         <v>507</v>
       </c>
@@ -11535,7 +11547,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="488" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A488" t="s">
         <v>509</v>
       </c>
@@ -11552,7 +11564,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="489" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A489" t="s">
         <v>510</v>
       </c>
@@ -11586,7 +11598,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="491" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A491" t="s">
         <v>512</v>
       </c>
@@ -11620,7 +11632,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="493" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A493" t="s">
         <v>514</v>
       </c>
@@ -11654,7 +11666,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="495" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A495" t="s">
         <v>516</v>
       </c>
@@ -11688,7 +11700,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="497" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A497" t="s">
         <v>518</v>
       </c>
@@ -11722,7 +11734,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="499" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A499" t="s">
         <v>520</v>
       </c>
@@ -11756,7 +11768,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="501" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A501" t="s">
         <v>522</v>
       </c>
@@ -11790,7 +11802,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="503" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A503" t="s">
         <v>524</v>
       </c>
@@ -11824,7 +11836,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="505" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A505" t="s">
         <v>526</v>
       </c>
@@ -11858,7 +11870,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="507" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="507" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A507" t="s">
         <v>528</v>
       </c>
@@ -11892,7 +11904,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="509" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="509" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A509" t="s">
         <v>530</v>
       </c>
@@ -11929,7 +11941,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="511" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="511" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A511" t="s">
         <v>532</v>
       </c>
@@ -11963,7 +11975,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="513" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="513" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A513" t="s">
         <v>534</v>
       </c>
@@ -11997,7 +12009,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="515" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="515" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A515" t="s">
         <v>536</v>
       </c>
@@ -12031,7 +12043,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="517" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="517" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A517" t="s">
         <v>538</v>
       </c>
@@ -12065,7 +12077,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="519" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="519" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A519" t="s">
         <v>540</v>
       </c>
@@ -12099,7 +12111,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="521" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="521" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A521" t="s">
         <v>542</v>
       </c>
@@ -12133,7 +12145,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="523" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="523" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A523" t="s">
         <v>544</v>
       </c>
@@ -12167,7 +12179,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="525" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="525" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A525" t="s">
         <v>546</v>
       </c>
@@ -12201,7 +12213,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="527" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="527" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A527" t="s">
         <v>548</v>
       </c>
@@ -12235,7 +12247,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="529" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="529" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A529" t="s">
         <v>550</v>
       </c>
@@ -12269,7 +12281,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="531" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="531" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A531" t="s">
         <v>552</v>
       </c>
@@ -12303,7 +12315,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="533" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="533" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A533" t="s">
         <v>554</v>
       </c>
@@ -12337,7 +12349,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="535" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="535" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A535" t="s">
         <v>556</v>
       </c>
@@ -12354,7 +12366,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="536" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="536" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A536" t="s">
         <v>557</v>
       </c>
@@ -12388,7 +12400,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="538" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="538" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A538" t="s">
         <v>559</v>
       </c>
@@ -12422,7 +12434,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="540" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="540" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A540" t="s">
         <v>561</v>
       </c>
@@ -12456,7 +12468,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="542" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="542" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A542" t="s">
         <v>563</v>
       </c>
@@ -12490,7 +12502,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="544" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="544" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A544" t="s">
         <v>567</v>
       </c>
@@ -12524,7 +12536,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="546" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="546" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A546" t="s">
         <v>569</v>
       </c>
@@ -12558,7 +12570,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="548" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="548" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A548" t="s">
         <v>571</v>
       </c>
@@ -12592,7 +12604,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="550" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="550" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A550" t="s">
         <v>573</v>
       </c>
@@ -12626,7 +12638,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="552" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="552" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A552" t="s">
         <v>575</v>
       </c>
@@ -12660,7 +12672,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="554" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="554" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A554" t="s">
         <v>577</v>
       </c>
@@ -12694,7 +12706,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="556" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="556" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A556" t="s">
         <v>579</v>
       </c>
@@ -12728,7 +12740,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="558" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="558" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A558" t="s">
         <v>581</v>
       </c>
@@ -12745,7 +12757,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="559" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="559" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A559" t="s">
         <v>582</v>
       </c>
@@ -12779,7 +12791,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="561" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="561" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A561" t="s">
         <v>584</v>
       </c>
@@ -12813,7 +12825,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="563" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="563" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A563" t="s">
         <v>586</v>
       </c>
@@ -12847,7 +12859,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="565" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="565" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A565" t="s">
         <v>588</v>
       </c>
@@ -12881,7 +12893,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="567" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="567" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A567" t="s">
         <v>590</v>
       </c>
@@ -12915,7 +12927,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="569" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="569" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A569" t="s">
         <v>592</v>
       </c>
@@ -12949,7 +12961,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="571" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="571" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A571" t="s">
         <v>594</v>
       </c>
@@ -12983,7 +12995,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="573" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="573" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A573" t="s">
         <v>596</v>
       </c>
@@ -13017,7 +13029,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="575" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="575" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A575" t="s">
         <v>598</v>
       </c>
@@ -13051,7 +13063,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="577" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="577" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A577" t="s">
         <v>600</v>
       </c>
@@ -13085,7 +13097,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="579" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="579" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A579" t="s">
         <v>602</v>
       </c>
@@ -13119,7 +13131,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="581" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="581" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A581" t="s">
         <v>604</v>
       </c>
@@ -13153,7 +13165,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="583" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="583" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A583" t="s">
         <v>606</v>
       </c>
@@ -13187,7 +13199,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="585" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="585" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A585" t="s">
         <v>608</v>
       </c>
@@ -13221,7 +13233,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="587" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="587" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A587" t="s">
         <v>610</v>
       </c>
@@ -13255,7 +13267,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="589" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="589" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A589" t="s">
         <v>612</v>
       </c>
@@ -13289,7 +13301,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="591" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="591" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A591" t="s">
         <v>614</v>
       </c>
@@ -13323,7 +13335,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="593" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="593" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A593" t="s">
         <v>616</v>
       </c>
@@ -13357,7 +13369,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="595" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="595" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A595" t="s">
         <v>618</v>
       </c>
@@ -13391,7 +13403,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="597" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="597" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A597" t="s">
         <v>620</v>
       </c>
@@ -13425,7 +13437,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="599" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="599" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A599" t="s">
         <v>622</v>
       </c>
@@ -13459,7 +13471,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="601" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="601" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A601" t="s">
         <v>624</v>
       </c>
@@ -13493,7 +13505,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="603" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="603" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A603" t="s">
         <v>626</v>
       </c>
@@ -13527,7 +13539,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="605" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="605" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A605" t="s">
         <v>628</v>
       </c>
@@ -13544,7 +13556,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="606" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="606" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A606" t="s">
         <v>629</v>
       </c>
@@ -13578,7 +13590,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="608" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="608" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A608" t="s">
         <v>631</v>
       </c>
@@ -13612,7 +13624,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="610" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="610" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A610" t="s">
         <v>633</v>
       </c>
@@ -13646,7 +13658,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="612" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="612" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A612" t="s">
         <v>635</v>
       </c>
@@ -13680,7 +13692,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="614" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="614" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A614" t="s">
         <v>637</v>
       </c>
@@ -13714,7 +13726,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="616" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="616" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A616" t="s">
         <v>639</v>
       </c>
@@ -13748,7 +13760,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="618" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="618" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A618" t="s">
         <v>641</v>
       </c>
@@ -13782,7 +13794,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="620" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="620" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A620" t="s">
         <v>643</v>
       </c>
@@ -13816,7 +13828,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="622" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="622" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A622" t="s">
         <v>645</v>
       </c>
@@ -13850,7 +13862,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="624" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="624" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A624" t="s">
         <v>647</v>
       </c>
@@ -13884,7 +13896,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="626" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="626" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A626" t="s">
         <v>649</v>
       </c>
@@ -13918,7 +13930,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="628" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="628" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A628" t="s">
         <v>651</v>
       </c>
@@ -13952,7 +13964,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="630" spans="1:5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="630" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A630" t="s">
         <v>653</v>
       </c>
@@ -13970,19 +13982,19 @@
       </c>
     </row>
     <row r="631" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A631" s="2" t="s">
+      <c r="A631" t="s">
         <v>654</v>
       </c>
-      <c r="B631" s="2">
-        <v>3</v>
-      </c>
-      <c r="C631" s="2" t="s">
+      <c r="B631">
+        <v>3</v>
+      </c>
+      <c r="C631" t="s">
         <v>88</v>
       </c>
-      <c r="D631" s="2" t="s">
+      <c r="D631" t="s">
         <v>564</v>
       </c>
-      <c r="E631" s="2" t="s">
+      <c r="E631" t="s">
         <v>565</v>
       </c>
     </row>

</xml_diff>